<commit_message>
spy, boomer 고유 미션 변경
</commit_message>
<xml_diff>
--- a/boomerMinigame.xlsx
+++ b/boomerMinigame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\endgame\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE905BC-6541-4EE6-83B8-4EA59C4D7740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573890C4-40CB-456D-B8DA-3E3159D3D4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="25620" windowHeight="11385" xr2:uid="{4791E7DD-F737-4612-93BC-85031DE34D39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4791E7DD-F737-4612-93BC-85031DE34D39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,22 @@
   </si>
   <si>
     <t>boomer_minigame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(min)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reducedTimePerMissionClear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(min)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -474,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1E530-3A6D-43E6-8931-A173E2FDDA13}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -485,9 +501,10 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,17 +514,23 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -517,8 +540,11 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -526,7 +552,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>